<commit_message>
Adding new manifesto runner script
</commit_message>
<xml_diff>
--- a/src/main/resources/valipop/inputs/proxy-scotland-population-JA/supporting-data/scaling-ob.xlsx
+++ b/src/main/resources/valipop/inputs/proxy-scotland-population-JA/supporting-data/scaling-ob.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsd4/OneDrive/cs/PhD/code/population-model/validated/src/main/resources/proxy-scotland-population-JA/supporting-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsd4/OneDrive/cs/PhD/code/population-model/src/main/resources/valipop/inputs/proxy-scotland-population-JA/supporting-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23161A9F-17AB-3C4E-AE49-8E9B299B862C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="6180" windowWidth="14400" windowHeight="9660" tabRatio="500"/>
+    <workbookView xWindow="21240" yWindow="2360" windowWidth="29360" windowHeight="22840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>15-19</t>
   </si>
@@ -52,22 +59,21 @@
   <si>
     <t>50-54</t>
   </si>
+  <si>
+    <t>EDI</t>
+  </si>
+  <si>
+    <t>SCOT (Scaled)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,18 +95,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -114,27 +114,27 @@
   </borders>
   <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -160,6 +160,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -427,19 +430,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="182" workbookViewId="0">
-      <selection activeCell="H12" sqref="B12:H19"/>
+    <sheetView tabSelected="1" zoomScale="182" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -665,6 +672,9 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B12" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>